<commit_message>
Optimization, Crew File Upload and Date formatting
</commit_message>
<xml_diff>
--- a/src/assets/static-content/Crews.xlsx
+++ b/src/assets/static-content/Crews.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Employee Number</t>
   </si>
@@ -33,6 +33,51 @@
   </si>
   <si>
     <t>Assigned Category</t>
+  </si>
+  <si>
+    <t>Employee's Base Location</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Departure Station Code</t>
+  </si>
+  <si>
+    <t>Arrival Station Code</t>
+  </si>
+  <si>
+    <t>Flight Number</t>
+  </si>
+  <si>
+    <t>Work Position</t>
+  </si>
+  <si>
+    <t>Phone Number</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Nationality</t>
+  </si>
+  <si>
+    <t>Passport Number</t>
+  </si>
+  <si>
+    <t>Passport Validity</t>
+  </si>
+  <si>
+    <t>NOK Name</t>
+  </si>
+  <si>
+    <t>NOK Contact Number</t>
+  </si>
+  <si>
+    <t>Medical Clearances</t>
   </si>
   <si>
     <r>
@@ -47,80 +92,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>deadhead crew</t>
+      <t>operating crew</t>
     </r>
-  </si>
-  <si>
-    <t>Employee's Base Location</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Departure Station Code</t>
-  </si>
-  <si>
-    <t>Arrival Station Code</t>
-  </si>
-  <si>
-    <t>Flight Number</t>
-  </si>
-  <si>
-    <t>Work Position</t>
-  </si>
-  <si>
-    <t>IGB22265</t>
-  </si>
-  <si>
-    <t>ANJALI SHARMA</t>
-  </si>
-  <si>
-    <t>CA</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>DEL</t>
-  </si>
-  <si>
-    <t>ANJALI.SHARMA@GOINDIGO.COM</t>
-  </si>
-  <si>
-    <t>CCU</t>
-  </si>
-  <si>
-    <t>6E-356</t>
-  </si>
-  <si>
-    <t>L1</t>
-  </si>
-  <si>
-    <t>Phone Number</t>
-  </si>
-  <si>
-    <t>Age</t>
-  </si>
-  <si>
-    <t>Gender</t>
-  </si>
-  <si>
-    <t>Nationality</t>
-  </si>
-  <si>
-    <t>Passport Number</t>
-  </si>
-  <si>
-    <t>Passport Validity</t>
-  </si>
-  <si>
-    <t>NOK Name</t>
-  </si>
-  <si>
-    <t>NOK Contact Number</t>
-  </si>
-  <si>
-    <t>Medical Clearances</t>
   </si>
 </sst>
 </file>
@@ -468,8 +441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,94 +478,61 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2">
-        <v>9876543210</v>
-      </c>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B2" s="1"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="1"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Pax and Crew Manifest Update
</commit_message>
<xml_diff>
--- a/src/assets/static-content/Crews.xlsx
+++ b/src/assets/static-content/Crews.xlsx
@@ -56,9 +56,6 @@
     <t>Phone Number</t>
   </si>
   <si>
-    <t>Age</t>
-  </si>
-  <si>
     <t>Gender</t>
   </si>
   <si>
@@ -94,6 +91,9 @@
       </rPr>
       <t>operating crew</t>
     </r>
+  </si>
+  <si>
+    <t>Date Of Birth(MM/DD/YYYY)</t>
   </si>
 </sst>
 </file>
@@ -442,7 +442,7 @@
   <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:K2"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,7 +467,7 @@
     <col min="19" max="19" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -478,7 +478,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -502,28 +502,28 @@
         <v>9</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
File Template Column type changed
</commit_message>
<xml_diff>
--- a/src/assets/static-content/Crews.xlsx
+++ b/src/assets/static-content/Crews.xlsx
@@ -442,7 +442,7 @@
   <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="P1" sqref="P1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,11 +457,11 @@
     <col min="9" max="9" width="9.140625" style="4"/>
     <col min="10" max="10" width="10.7109375" customWidth="1"/>
     <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.7109375" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" style="4" customWidth="1"/>
     <col min="13" max="13" width="12.5703125" customWidth="1"/>
     <col min="14" max="14" width="14.85546875" customWidth="1"/>
     <col min="15" max="15" width="16.140625" customWidth="1"/>
-    <col min="16" max="16" width="15.5703125" customWidth="1"/>
+    <col min="16" max="16" width="15.5703125" style="4" customWidth="1"/>
     <col min="17" max="17" width="18.5703125" customWidth="1"/>
     <col min="18" max="18" width="14.42578125" customWidth="1"/>
     <col min="19" max="19" width="17.85546875" customWidth="1"/>
@@ -501,7 +501,7 @@
       <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="3" t="s">
         <v>18</v>
       </c>
       <c r="M1" s="1" t="s">
@@ -513,7 +513,7 @@
       <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="3" t="s">
         <v>13</v>
       </c>
       <c r="Q1" s="1" t="s">

</xml_diff>